<commit_message>
Working on deep learning
</commit_message>
<xml_diff>
--- a/Important_links.xlsx
+++ b/Important_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaymittal/Monash/Summer_Vacation/GitHub/Deep-Learning-Material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB4A90C-774D-E04C-AAE6-15BFFCD5466B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D3A384-5E79-124E-864F-CFCA55341771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="1500" windowWidth="28800" windowHeight="17440" activeTab="1" xr2:uid="{FD4613A6-FE53-4D4C-8400-58CEE97B25AB}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Working Deep Learning Algorithm
</commit_message>
<xml_diff>
--- a/Important_links.xlsx
+++ b/Important_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaymittal/Monash/Summer_Vacation/GitHub/Deep-Learning-Material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D3A384-5E79-124E-864F-CFCA55341771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB15D5FF-E85F-4F4F-B8FC-BB7FC572D47A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="1500" windowWidth="28800" windowHeight="17440" activeTab="1" xr2:uid="{FD4613A6-FE53-4D4C-8400-58CEE97B25AB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Import Wesbite for deep learning</t>
   </si>
@@ -82,6 +82,30 @@
   </si>
   <si>
     <t>Regularization</t>
+  </si>
+  <si>
+    <t>Activation Functon</t>
+  </si>
+  <si>
+    <t>Variants of Relu</t>
+  </si>
+  <si>
+    <t>Weight Initialisation Technique</t>
+  </si>
+  <si>
+    <t>https://www.deeplearning.ai/ai-notes/initialization/index.html</t>
+  </si>
+  <si>
+    <t>Xavier</t>
+  </si>
+  <si>
+    <t>Batch Normalisation</t>
+  </si>
+  <si>
+    <t>Optimiser</t>
+  </si>
+  <si>
+    <t>Exponentially Weighted Moving Average</t>
   </si>
 </sst>
 </file>
@@ -472,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D93727A-96BB-0740-9526-749377257D0D}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A1:A1048576"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -504,9 +528,15 @@
         <v>2</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{DFDC96EB-36FA-C344-8BC7-9115A64CD539}"/>
+    <hyperlink ref="B5" r:id="rId2" xr:uid="{9CE2D193-3C95-2D43-BC53-1BAC48056763}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -514,10 +544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A632D425-0AE6-B94E-8D3D-AE689FD971F0}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,6 +605,41 @@
         <v>14</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Working with deep learning material
</commit_message>
<xml_diff>
--- a/Important_links.xlsx
+++ b/Important_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaymittal/Monash/Summer_Vacation/GitHub/Deep-Learning-Material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EDEF051-A6C4-BA42-8CC7-8B9516C21AD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68870CDA-15B9-F24C-A0EB-413C131B9758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="1500" windowWidth="28800" windowHeight="17440" activeTab="1" xr2:uid="{FD4613A6-FE53-4D4C-8400-58CEE97B25AB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>Import Wesbite for deep learning</t>
   </si>
@@ -109,6 +109,15 @@
   </si>
   <si>
     <t>SGD with Momentum</t>
+  </si>
+  <si>
+    <t>optimiser</t>
+  </si>
+  <si>
+    <t>Nesterov Accelerated Gradient (NAG)</t>
+  </si>
+  <si>
+    <t>AdaGrad</t>
   </si>
 </sst>
 </file>
@@ -547,10 +556,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A632D425-0AE6-B94E-8D3D-AE689FD971F0}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,14 +647,33 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>23</v>
+      </c>
+      <c r="B18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on the transformer
</commit_message>
<xml_diff>
--- a/Important_links.xlsx
+++ b/Important_links.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vinaymittal/Monash/Summer_Vacation/GitHub/Deep-Learning-Material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFAA8AC-5F27-2548-B89A-EB5743AC5CA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCD410F-FAE3-2042-991E-8D8D27916D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3440" yWindow="1500" windowWidth="28800" windowHeight="17440" activeTab="1" xr2:uid="{FD4613A6-FE53-4D4C-8400-58CEE97B25AB}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="39">
   <si>
     <t>Import Wesbite for deep learning</t>
   </si>
@@ -148,6 +148,12 @@
   </si>
   <si>
     <t>Attention Mechanism</t>
+  </si>
+  <si>
+    <t>Bahndau Vs luong</t>
+  </si>
+  <si>
+    <t>Tranformers</t>
   </si>
 </sst>
 </file>
@@ -586,10 +592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A632D425-0AE6-B94E-8D3D-AE689FD971F0}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -756,6 +762,16 @@
         <v>36</v>
       </c>
     </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>